<commit_message>
ready to rollout the presentations
</commit_message>
<xml_diff>
--- a/EDA/Indicators_New_structures.xlsx
+++ b/EDA/Indicators_New_structures.xlsx
@@ -572,65 +572,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -670,65 +646,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -783,28 +735,28 @@
         <v>20</v>
       </c>
       <c r="M4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O4" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="P4" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q4" t="n">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="R4" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="S4" t="n">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="T4" t="n">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
@@ -853,34 +805,34 @@
         <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L5" t="n">
         <v>20</v>
       </c>
       <c r="M5" t="n">
+        <v>27</v>
+      </c>
+      <c r="N5" t="n">
         <v>25</v>
       </c>
-      <c r="N5" t="n">
-        <v>22</v>
-      </c>
       <c r="O5" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="P5" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="R5" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="S5" t="n">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="T5" t="n">
-        <v>92</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -929,34 +881,34 @@
         <v>100</v>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="N6" t="n">
         <v>3</v>
       </c>
       <c r="O6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P6" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q6" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="R6" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="S6" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="T6" t="n">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
@@ -1005,34 +957,34 @@
         <v>100</v>
       </c>
       <c r="K7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="P7" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R7" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="S7" t="n">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="T7" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8">
@@ -1081,34 +1033,34 @@
         <v>100</v>
       </c>
       <c r="K8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>4</v>
+      </c>
+      <c r="P8" t="n">
         <v>2</v>
       </c>
-      <c r="M8" t="n">
-        <v>7</v>
-      </c>
-      <c r="N8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O8" t="n">
-        <v>27</v>
-      </c>
-      <c r="P8" t="n">
-        <v>20</v>
-      </c>
       <c r="Q8" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="R8" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="S8" t="n">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="T8" t="n">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
@@ -1163,28 +1115,28 @@
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N9" t="n">
         <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q9" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="R9" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="S9" t="n">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="T9" t="n">
-        <v>99</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10">
@@ -1245,22 +1197,22 @@
         <v>1</v>
       </c>
       <c r="O10" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" t="n">
         <v>3</v>
       </c>
-      <c r="P10" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>5</v>
-      </c>
-      <c r="R10" t="n">
-        <v>5</v>
-      </c>
       <c r="S10" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="T10" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -1309,34 +1261,34 @@
         <v>40</v>
       </c>
       <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" t="n">
+        <v>2</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="n">
         <v>3</v>
       </c>
-      <c r="L11" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" t="n">
-        <v>3</v>
-      </c>
-      <c r="N11" t="n">
-        <v>1</v>
-      </c>
-      <c r="O11" t="n">
-        <v>7</v>
-      </c>
-      <c r="P11" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>9</v>
-      </c>
       <c r="R11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S11" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="T11" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
@@ -1385,34 +1337,34 @@
         <v>100</v>
       </c>
       <c r="K12" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L12" t="n">
         <v>20</v>
       </c>
       <c r="M12" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N12" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O12" t="n">
+        <v>22</v>
+      </c>
+      <c r="P12" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q12" t="n">
         <v>23</v>
       </c>
-      <c r="P12" t="n">
-        <v>21</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>28</v>
-      </c>
       <c r="R12" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S12" t="n">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="T12" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -1461,31 +1413,31 @@
         <v>12</v>
       </c>
       <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1</v>
+      </c>
+      <c r="O13" t="n">
         <v>2</v>
-      </c>
-      <c r="L13" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2</v>
-      </c>
-      <c r="N13" t="n">
-        <v>2</v>
-      </c>
-      <c r="O13" t="n">
-        <v>3</v>
       </c>
       <c r="P13" t="n">
         <v>2</v>
       </c>
       <c r="Q13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S13" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="T13" t="n">
         <v>10</v>
@@ -1549,22 +1501,22 @@
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P14" t="n">
         <v>1</v>
       </c>
       <c r="Q14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1613,10 +1565,10 @@
         <v>100</v>
       </c>
       <c r="K15" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L15" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M15" t="n">
         <v>21</v>
@@ -1625,22 +1577,22 @@
         <v>20</v>
       </c>
       <c r="O15" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P15" t="n">
         <v>21</v>
       </c>
       <c r="Q15" t="n">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="R15" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="S15" t="n">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="T15" t="n">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16">
@@ -1689,34 +1641,34 @@
         <v>100</v>
       </c>
       <c r="K16" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L16" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M16" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N16" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O16" t="n">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="P16" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="Q16" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="R16" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="S16" t="n">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="T16" t="n">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -1765,22 +1717,22 @@
         <v>100</v>
       </c>
       <c r="K17" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L17" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M17" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="N17" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="O17" t="n">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="P17" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q17" t="n">
         <v>44</v>
@@ -1789,10 +1741,10 @@
         <v>32</v>
       </c>
       <c r="S17" t="n">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="T17" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -1853,19 +1805,19 @@
         <v>1</v>
       </c>
       <c r="O18" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q18" t="n">
         <v>4</v>
       </c>
       <c r="R18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T18" t="n">
         <v>9</v>
@@ -1917,34 +1869,34 @@
         <v>100</v>
       </c>
       <c r="K19" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L19" t="n">
         <v>20</v>
       </c>
       <c r="M19" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="N19" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O19" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="P19" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="Q19" t="n">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="R19" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="S19" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="T19" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -1999,28 +1951,28 @@
         <v>7</v>
       </c>
       <c r="M20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O20" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="P20" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q20" t="n">
         <v>11</v>
       </c>
       <c r="R20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S20" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="T20" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -2060,65 +2012,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -2167,34 +2095,34 @@
         <v>100</v>
       </c>
       <c r="K22" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="L22" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="M22" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N22" t="n">
+        <v>21</v>
+      </c>
+      <c r="O22" t="n">
         <v>27</v>
       </c>
-      <c r="O22" t="n">
-        <v>39</v>
-      </c>
       <c r="P22" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q22" t="n">
         <v>31</v>
       </c>
-      <c r="Q22" t="n">
-        <v>40</v>
-      </c>
       <c r="R22" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="S22" t="n">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="T22" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
@@ -2243,34 +2171,34 @@
         <v>100</v>
       </c>
       <c r="K23" t="n">
+        <v>22</v>
+      </c>
+      <c r="L23" t="n">
+        <v>22</v>
+      </c>
+      <c r="M23" t="n">
+        <v>31</v>
+      </c>
+      <c r="N23" t="n">
+        <v>31</v>
+      </c>
+      <c r="O23" t="n">
+        <v>35</v>
+      </c>
+      <c r="P23" t="n">
         <v>21</v>
       </c>
-      <c r="L23" t="n">
-        <v>20</v>
-      </c>
-      <c r="M23" t="n">
-        <v>24</v>
-      </c>
-      <c r="N23" t="n">
-        <v>22</v>
-      </c>
-      <c r="O23" t="n">
-        <v>30</v>
-      </c>
-      <c r="P23" t="n">
-        <v>24</v>
-      </c>
       <c r="Q23" t="n">
+        <v>44</v>
+      </c>
+      <c r="R23" t="n">
         <v>43</v>
       </c>
-      <c r="R23" t="n">
-        <v>42</v>
-      </c>
       <c r="S23" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="T23" t="n">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
@@ -2331,22 +2259,22 @@
         <v>20</v>
       </c>
       <c r="O24" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P24" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q24" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R24" t="n">
         <v>22</v>
       </c>
       <c r="S24" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="T24" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25">
@@ -2401,28 +2329,28 @@
         <v>20</v>
       </c>
       <c r="M25" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N25" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O25" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P25" t="n">
         <v>21</v>
       </c>
       <c r="Q25" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="R25" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="S25" t="n">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="T25" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26">
@@ -2477,28 +2405,28 @@
         <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N26" t="n">
+        <v>1</v>
+      </c>
+      <c r="O26" t="n">
         <v>2</v>
       </c>
-      <c r="O26" t="n">
-        <v>5</v>
-      </c>
       <c r="P26" t="n">
         <v>1</v>
       </c>
       <c r="Q26" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="R26" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="S26" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="T26" t="n">
-        <v>98</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27">
@@ -2547,10 +2475,10 @@
         <v>200</v>
       </c>
       <c r="K27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M27" t="n">
         <v>3</v>
@@ -2559,22 +2487,22 @@
         <v>2</v>
       </c>
       <c r="O27" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="P27" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q27" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="R27" t="n">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="S27" t="n">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="T27" t="n">
-        <v>172</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28">
@@ -2623,34 +2551,34 @@
         <v>200</v>
       </c>
       <c r="K28" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="L28" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M28" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="N28" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="O28" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="P28" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="Q28" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="R28" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="S28" t="n">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="T28" t="n">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29">
@@ -2705,28 +2633,28 @@
         <v>1</v>
       </c>
       <c r="M29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N29" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O29" t="n">
+        <v>11</v>
+      </c>
+      <c r="P29" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q29" t="n">
         <v>18</v>
       </c>
-      <c r="P29" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>23</v>
-      </c>
       <c r="R29" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="S29" t="n">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="T29" t="n">
-        <v>95</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30">
@@ -2793,16 +2721,16 @@
         <v>1</v>
       </c>
       <c r="Q30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S30" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="T30" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
@@ -2872,13 +2800,13 @@
         <v>3</v>
       </c>
       <c r="R31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S31" t="n">
         <v>8</v>
       </c>
       <c r="T31" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -2939,22 +2867,22 @@
         <v>20</v>
       </c>
       <c r="O32" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="P32" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="Q32" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="R32" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="S32" t="n">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="T32" t="n">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33">
@@ -3003,7 +2931,7 @@
         <v>100</v>
       </c>
       <c r="K33" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L33" t="n">
         <v>20</v>
@@ -3012,25 +2940,25 @@
         <v>23</v>
       </c>
       <c r="N33" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O33" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P33" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q33" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="R33" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="S33" t="n">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="T33" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
@@ -3079,34 +3007,34 @@
         <v>100</v>
       </c>
       <c r="K34" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L34" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="M34" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="N34" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="O34" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="P34" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q34" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="R34" t="n">
         <v>23</v>
       </c>
       <c r="S34" t="n">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="T34" t="n">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35">
@@ -3164,25 +3092,25 @@
         <v>2</v>
       </c>
       <c r="N35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O35" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="P35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>28</v>
+      </c>
+      <c r="R35" t="n">
         <v>7</v>
       </c>
-      <c r="Q35" t="n">
-        <v>33</v>
-      </c>
-      <c r="R35" t="n">
-        <v>12</v>
-      </c>
       <c r="S35" t="n">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="T35" t="n">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36">
@@ -3231,34 +3159,34 @@
         <v>200</v>
       </c>
       <c r="K36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N36" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O36" t="n">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="P36" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="Q36" t="n">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="R36" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="S36" t="n">
-        <v>121</v>
+        <v>80</v>
       </c>
       <c r="T36" t="n">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37">
@@ -3307,34 +3235,34 @@
         <v>200</v>
       </c>
       <c r="K37" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M37" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="N37" t="n">
         <v>6</v>
       </c>
       <c r="O37" t="n">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="P37" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="Q37" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="R37" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="S37" t="n">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="T37" t="n">
-        <v>137</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38">
@@ -3383,34 +3311,34 @@
         <v>150</v>
       </c>
       <c r="K38" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="L38" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="M38" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="N38" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="O38" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="P38" t="n">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="Q38" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="R38" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="S38" t="n">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="T38" t="n">
-        <v>79</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39">
@@ -3459,34 +3387,34 @@
         <v>100</v>
       </c>
       <c r="K39" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L39" t="n">
         <v>20</v>
       </c>
       <c r="M39" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N39" t="n">
         <v>21</v>
       </c>
       <c r="O39" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P39" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q39" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R39" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="S39" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T39" t="n">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40">
@@ -3535,34 +3463,34 @@
         <v>100</v>
       </c>
       <c r="K40" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L40" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M40" t="n">
+        <v>25</v>
+      </c>
+      <c r="N40" t="n">
+        <v>24</v>
+      </c>
+      <c r="O40" t="n">
+        <v>26</v>
+      </c>
+      <c r="P40" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>28</v>
+      </c>
+      <c r="R40" t="n">
         <v>23</v>
       </c>
-      <c r="N40" t="n">
-        <v>20</v>
-      </c>
-      <c r="O40" t="n">
-        <v>38</v>
-      </c>
-      <c r="P40" t="n">
-        <v>34</v>
-      </c>
-      <c r="Q40" t="n">
-        <v>48</v>
-      </c>
-      <c r="R40" t="n">
-        <v>30</v>
-      </c>
       <c r="S40" t="n">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="T40" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41">
@@ -3611,34 +3539,34 @@
         <v>100</v>
       </c>
       <c r="K41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L41" t="n">
         <v>1</v>
       </c>
       <c r="M41" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N41" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O41" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="P41" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q41" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="R41" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="S41" t="n">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="T41" t="n">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42">
@@ -3693,28 +3621,28 @@
         <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N42" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O42" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="P42" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="Q42" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="R42" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="S42" t="n">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="T42" t="n">
-        <v>77</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43">
@@ -3763,34 +3691,34 @@
         <v>100</v>
       </c>
       <c r="K43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M43" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O43" t="n">
+        <v>3</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>21</v>
+      </c>
+      <c r="R43" t="n">
         <v>18</v>
       </c>
-      <c r="P43" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>20</v>
-      </c>
-      <c r="R43" t="n">
-        <v>4</v>
-      </c>
       <c r="S43" t="n">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="T43" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44">
@@ -3839,34 +3767,34 @@
         <v>100</v>
       </c>
       <c r="K44" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L44" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M44" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="N44" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="O44" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="P44" t="n">
         <v>22</v>
       </c>
       <c r="Q44" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="R44" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S44" t="n">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="T44" t="n">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45">
@@ -3933,16 +3861,16 @@
         <v>20</v>
       </c>
       <c r="Q45" t="n">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="R45" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="S45" t="n">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="T45" t="n">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46">
@@ -3997,28 +3925,28 @@
         <v>2</v>
       </c>
       <c r="M46" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N46" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O46" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="P46" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="Q46" t="n">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="R46" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="S46" t="n">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="T46" t="n">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47">
@@ -4070,31 +3998,31 @@
         <v>2</v>
       </c>
       <c r="L47" t="n">
+        <v>1</v>
+      </c>
+      <c r="M47" t="n">
+        <v>4</v>
+      </c>
+      <c r="N47" t="n">
         <v>2</v>
       </c>
-      <c r="M47" t="n">
-        <v>2</v>
-      </c>
-      <c r="N47" t="n">
-        <v>1</v>
-      </c>
       <c r="O47" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="P47" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q47" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="R47" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="S47" t="n">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="T47" t="n">
-        <v>198</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48">
@@ -4143,34 +4071,34 @@
         <v>200</v>
       </c>
       <c r="K48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N48" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O48" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P48" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="Q48" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R48" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S48" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="T48" t="n">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49">
@@ -4219,34 +4147,34 @@
         <v>200</v>
       </c>
       <c r="K49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L49" t="n">
         <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N49" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O49" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="P49" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="Q49" t="n">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="R49" t="n">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="S49" t="n">
-        <v>154</v>
+        <v>97</v>
       </c>
       <c r="T49" t="n">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50">
@@ -4295,34 +4223,34 @@
         <v>200</v>
       </c>
       <c r="K50" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M50" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N50" t="n">
         <v>1</v>
       </c>
       <c r="O50" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P50" t="n">
         <v>4</v>
       </c>
       <c r="Q50" t="n">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="R50" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="S50" t="n">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="T50" t="n">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51">
@@ -4371,34 +4299,34 @@
         <v>200</v>
       </c>
       <c r="K51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M51" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="N51" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O51" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="P51" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="Q51" t="n">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="R51" t="n">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="S51" t="n">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="T51" t="n">
-        <v>199</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52">
@@ -4438,65 +4366,41 @@
           <t>-</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="T52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0</v>
+      </c>
+      <c r="T52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -4545,34 +4449,34 @@
         <v>20000</v>
       </c>
       <c r="K53" t="n">
+        <v>500</v>
+      </c>
+      <c r="L53" t="n">
+        <v>500</v>
+      </c>
+      <c r="M53" t="n">
         <v>501</v>
       </c>
-      <c r="L53" t="n">
+      <c r="N53" t="n">
+        <v>500</v>
+      </c>
+      <c r="O53" t="n">
         <v>501</v>
       </c>
-      <c r="M53" t="n">
-        <v>513</v>
-      </c>
-      <c r="N53" t="n">
-        <v>509</v>
-      </c>
-      <c r="O53" t="n">
-        <v>838</v>
-      </c>
       <c r="P53" t="n">
-        <v>736</v>
+        <v>501</v>
       </c>
       <c r="Q53" t="n">
-        <v>1101</v>
+        <v>856</v>
       </c>
       <c r="R53" t="n">
-        <v>754</v>
+        <v>745</v>
       </c>
       <c r="S53" t="n">
-        <v>19047</v>
+        <v>19642</v>
       </c>
       <c r="T53" t="n">
-        <v>19500</v>
+        <v>19754</v>
       </c>
     </row>
     <row r="54">
@@ -4621,34 +4525,34 @@
         <v>100</v>
       </c>
       <c r="K54" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L54" t="n">
         <v>20</v>
       </c>
       <c r="M54" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N54" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O54" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P54" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q54" t="n">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="R54" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="S54" t="n">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="T54" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55">
@@ -4697,34 +4601,34 @@
         <v>20000</v>
       </c>
       <c r="K55" t="n">
-        <v>1138</v>
+        <v>1359</v>
       </c>
       <c r="L55" t="n">
-        <v>732</v>
+        <v>1309</v>
       </c>
       <c r="M55" t="n">
-        <v>1334</v>
+        <v>2208</v>
       </c>
       <c r="N55" t="n">
-        <v>855</v>
+        <v>913</v>
       </c>
       <c r="O55" t="n">
-        <v>1497</v>
+        <v>2857</v>
       </c>
       <c r="P55" t="n">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="Q55" t="n">
-        <v>3049</v>
+        <v>3468</v>
       </c>
       <c r="R55" t="n">
-        <v>2094</v>
+        <v>1713</v>
       </c>
       <c r="S55" t="n">
-        <v>14982</v>
+        <v>12108</v>
       </c>
       <c r="T55" t="n">
-        <v>16987</v>
+        <v>16735</v>
       </c>
     </row>
     <row r="56">
@@ -4773,34 +4677,34 @@
         <v>20000</v>
       </c>
       <c r="K56" t="n">
-        <v>1084</v>
+        <v>767</v>
       </c>
       <c r="L56" t="n">
-        <v>757</v>
+        <v>641</v>
       </c>
       <c r="M56" t="n">
-        <v>1902</v>
+        <v>1139</v>
       </c>
       <c r="N56" t="n">
-        <v>1654</v>
+        <v>1062</v>
       </c>
       <c r="O56" t="n">
-        <v>3493</v>
+        <v>2191</v>
       </c>
       <c r="P56" t="n">
-        <v>614</v>
+        <v>1775</v>
       </c>
       <c r="Q56" t="n">
-        <v>4190</v>
+        <v>6765</v>
       </c>
       <c r="R56" t="n">
-        <v>3928</v>
+        <v>681</v>
       </c>
       <c r="S56" t="n">
-        <v>11331</v>
+        <v>11138</v>
       </c>
       <c r="T56" t="n">
-        <v>15047</v>
+        <v>17841</v>
       </c>
     </row>
     <row r="57">
@@ -4849,34 +4753,34 @@
         <v>100</v>
       </c>
       <c r="K57" t="n">
+        <v>22</v>
+      </c>
+      <c r="L57" t="n">
+        <v>21</v>
+      </c>
+      <c r="M57" t="n">
         <v>23</v>
       </c>
-      <c r="L57" t="n">
-        <v>22</v>
-      </c>
-      <c r="M57" t="n">
-        <v>27</v>
-      </c>
       <c r="N57" t="n">
+        <v>20</v>
+      </c>
+      <c r="O57" t="n">
+        <v>25</v>
+      </c>
+      <c r="P57" t="n">
         <v>23</v>
       </c>
-      <c r="O57" t="n">
-        <v>29</v>
-      </c>
-      <c r="P57" t="n">
-        <v>29</v>
-      </c>
       <c r="Q57" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="R57" t="n">
         <v>32</v>
       </c>
       <c r="S57" t="n">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="T57" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58">
@@ -4937,22 +4841,22 @@
         <v>1</v>
       </c>
       <c r="O58" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q58" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="R58" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="S58" t="n">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="T58" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59">
@@ -5001,34 +4905,34 @@
         <v>100</v>
       </c>
       <c r="K59" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M59" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="N59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O59" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="P59" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="Q59" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="R59" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="S59" t="n">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="T59" t="n">
-        <v>68</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>